<commit_message>
Ajout date de création
MS sur date de création du RDV b46a3338cdb44285bac1ca418442b3b63435dcea
</commit_message>
<xml_diff>
--- a/feature/add-created-date/ig/StructureDefinition-FrAppointmentSAS.xlsx
+++ b/feature/add-created-date/ig/StructureDefinition-FrAppointmentSAS.xlsx
@@ -9,6 +9,9 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AJ$97</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -54,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-30T07:24:56+00:00</t>
+    <t>2025-06-30T07:28:14+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1629,6 +1632,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1959,7 +1977,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>29</v>
       </c>
@@ -2059,7 +2077,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>79</v>
       </c>
@@ -2161,7 +2179,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>87</v>
       </c>
@@ -2261,7 +2279,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>94</v>
       </c>
@@ -2363,7 +2381,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>100</v>
       </c>
@@ -2465,7 +2483,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>109</v>
       </c>
@@ -2567,7 +2585,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>116</v>
       </c>
@@ -2669,7 +2687,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>123</v>
       </c>
@@ -2769,7 +2787,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>132</v>
       </c>
@@ -2871,7 +2889,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>137</v>
       </c>
@@ -2971,7 +2989,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>143</v>
       </c>
@@ -3071,7 +3089,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
         <v>146</v>
       </c>
@@ -3173,7 +3191,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>153</v>
       </c>
@@ -3271,7 +3289,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
         <v>161</v>
       </c>
@@ -3373,7 +3391,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
         <v>164</v>
       </c>
@@ -3473,7 +3491,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
         <v>166</v>
       </c>
@@ -3575,7 +3593,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
         <v>172</v>
       </c>
@@ -3677,7 +3695,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
         <v>179</v>
       </c>
@@ -3779,7 +3797,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
         <v>188</v>
       </c>
@@ -3881,7 +3899,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
         <v>195</v>
       </c>
@@ -3981,7 +3999,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
         <v>197</v>
       </c>
@@ -4083,7 +4101,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
         <v>199</v>
       </c>
@@ -4187,7 +4205,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
         <v>209</v>
       </c>
@@ -4291,7 +4309,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
         <v>219</v>
       </c>
@@ -4391,7 +4409,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
         <v>221</v>
       </c>
@@ -4493,7 +4511,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
         <v>223</v>
       </c>
@@ -4597,7 +4615,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
         <v>231</v>
       </c>
@@ -4697,7 +4715,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
         <v>233</v>
       </c>
@@ -4799,7 +4817,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
         <v>235</v>
       </c>
@@ -4903,7 +4921,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
         <v>243</v>
       </c>
@@ -5005,7 +5023,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
         <v>249</v>
       </c>
@@ -5109,7 +5127,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
         <v>256</v>
       </c>
@@ -5213,7 +5231,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
         <v>262</v>
       </c>
@@ -5317,7 +5335,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
         <v>270</v>
       </c>
@@ -5421,7 +5439,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
         <v>277</v>
       </c>
@@ -5525,7 +5543,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
         <v>285</v>
       </c>
@@ -5627,7 +5645,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
         <v>292</v>
       </c>
@@ -5729,7 +5747,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
         <v>300</v>
       </c>
@@ -5831,7 +5849,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
         <v>308</v>
       </c>
@@ -5933,7 +5951,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
         <v>314</v>
       </c>
@@ -6037,7 +6055,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
         <v>319</v>
       </c>
@@ -6137,7 +6155,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
         <v>322</v>
       </c>
@@ -6237,7 +6255,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
         <v>323</v>
       </c>
@@ -6339,7 +6357,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
         <v>324</v>
       </c>
@@ -6443,7 +6461,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
         <v>325</v>
       </c>
@@ -6547,7 +6565,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
         <v>326</v>
       </c>
@@ -6651,7 +6669,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
         <v>327</v>
       </c>
@@ -6753,7 +6771,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
         <v>328</v>
       </c>
@@ -6855,7 +6873,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
         <v>329</v>
       </c>
@@ -6957,7 +6975,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
         <v>330</v>
       </c>
@@ -7059,7 +7077,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
         <v>336</v>
       </c>
@@ -7159,7 +7177,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
         <v>342</v>
       </c>
@@ -7259,7 +7277,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
         <v>346</v>
       </c>
@@ -7359,7 +7377,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
         <v>351</v>
       </c>
@@ -7459,7 +7477,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
         <v>355</v>
       </c>
@@ -7559,7 +7577,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
         <v>359</v>
       </c>
@@ -7661,7 +7679,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
         <v>364</v>
       </c>
@@ -7763,7 +7781,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
         <v>369</v>
       </c>
@@ -7865,7 +7883,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
         <v>374</v>
       </c>
@@ -7967,7 +7985,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
         <v>377</v>
       </c>
@@ -8069,7 +8087,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
         <v>381</v>
       </c>
@@ -8171,7 +8189,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
         <v>386</v>
       </c>
@@ -8273,7 +8291,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
         <v>389</v>
       </c>
@@ -8375,7 +8393,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
         <v>394</v>
       </c>
@@ -8477,7 +8495,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
         <v>398</v>
       </c>
@@ -8496,7 +8514,7 @@
         <v>80</v>
       </c>
       <c r="H66" t="s" s="2">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="I66" t="s" s="2">
         <v>72</v>
@@ -8579,7 +8597,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
         <v>403</v>
       </c>
@@ -8681,7 +8699,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
         <v>407</v>
       </c>
@@ -8783,7 +8801,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
         <v>410</v>
       </c>
@@ -8885,7 +8903,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
         <v>415</v>
       </c>
@@ -8985,7 +9003,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
         <v>420</v>
       </c>
@@ -9085,7 +9103,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
         <v>421</v>
       </c>
@@ -9187,7 +9205,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
         <v>422</v>
       </c>
@@ -9291,7 +9309,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
         <v>427</v>
       </c>
@@ -9393,7 +9411,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
         <v>433</v>
       </c>
@@ -9495,7 +9513,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
         <v>437</v>
       </c>
@@ -9595,7 +9613,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
         <v>438</v>
       </c>
@@ -9697,7 +9715,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
         <v>439</v>
       </c>
@@ -9799,7 +9817,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
         <v>440</v>
       </c>
@@ -9901,7 +9919,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
         <v>441</v>
       </c>
@@ -10003,7 +10021,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
         <v>442</v>
       </c>
@@ -10103,7 +10121,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
         <v>443</v>
       </c>
@@ -10205,7 +10223,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
         <v>444</v>
       </c>
@@ -10309,7 +10327,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
         <v>445</v>
       </c>
@@ -10413,7 +10431,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
         <v>446</v>
       </c>
@@ -10513,7 +10531,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
         <v>447</v>
       </c>
@@ -10615,7 +10633,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
         <v>448</v>
       </c>
@@ -10719,7 +10737,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
         <v>450</v>
       </c>
@@ -10823,7 +10841,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
         <v>451</v>
       </c>
@@ -10927,7 +10945,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
         <v>453</v>
       </c>
@@ -11029,7 +11047,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
         <v>454</v>
       </c>
@@ -11131,7 +11149,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
         <v>455</v>
       </c>
@@ -11233,7 +11251,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
         <v>456</v>
       </c>
@@ -11335,7 +11353,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
         <v>457</v>
       </c>
@@ -11437,7 +11455,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
         <v>462</v>
       </c>
@@ -11539,7 +11557,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
         <v>468</v>
       </c>
@@ -11641,7 +11659,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
         <v>471</v>
       </c>
@@ -11744,6 +11762,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AJ97">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI96">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>